<commit_message>
complete 50 results for 15M
</commit_message>
<xml_diff>
--- a/Results/20231224 Revision_Simulated_Tornado_15M.xlsx
+++ b/Results/20231224 Revision_Simulated_Tornado_15M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306147E9-6C0F-404A-BF5E-89B5C6D08832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524CC5E4-D693-4D95-944F-1086A736CA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="39">
   <si>
     <t>Budget :</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>fixedpointB</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -643,7 +655,7 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,15 +769,15 @@
       </c>
       <c r="K11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="L11">
         <f ca="1">INDEX(Table1[coordinate_x],MATCH(K11,Table1[Block ID],0))</f>
-        <v>-94.512</v>
+        <v>-94.504999999999995</v>
       </c>
       <c r="M11">
         <f ca="1">INDEX(Table1[coordinate_y],MATCH(K11,Table1[Block ID],0))</f>
-        <v>37.06</v>
+        <v>37.091999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -783,11 +795,11 @@
       </c>
       <c r="L12">
         <f ca="1">L11*54.6</f>
-        <v>-5160.3552</v>
+        <v>-5159.973</v>
       </c>
       <c r="M12">
         <f ca="1">M11*69</f>
-        <v>2557.1400000000003</v>
+        <v>2559.348</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -871,7 +883,7 @@
       </c>
       <c r="O16">
         <f ca="1">SQRT((L16-$L$12)^2+(M16-$M$12)^2)</f>
-        <v>1.0772132379428725</v>
+        <v>1.4985585874433502</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -912,7 +924,7 @@
       </c>
       <c r="O17">
         <f ca="1">SQRT((L17-$L$12)^2+(M17-$M$12)^2)</f>
-        <v>1.7264410676299904</v>
+        <v>1.0558745380016294</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -952,8 +964,8 @@
         <v>2557.9680000000003</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O17:O21" ca="1" si="0">SQRT((L18-$L$12)^2+(M18-$M$12)^2)</f>
-        <v>0.91195440675505623</v>
+        <f t="shared" ref="O18:O19" ca="1" si="0">SQRT((L18-$L$12)^2+(M18-$M$12)^2)</f>
+        <v>1.3799999999996544</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -994,7 +1006,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7039163586677033</v>
+        <v>1.8474569007152806</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -1035,7 +1047,7 @@
       </c>
       <c r="O20">
         <f ca="1">SQRT((L20-$L$12)^2+(M20-$M$12)^2)</f>
-        <v>2.1883555469806457</v>
+        <v>3.4769380840045288</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1076,7 +1088,7 @@
       </c>
       <c r="O21">
         <f ca="1">SQRT((L21-$L$12)^2+(M21-$M$12)^2)</f>
-        <v>1.0950729838695981</v>
+        <v>2.1997386208369334</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1117,7 +1129,7 @@
       </c>
       <c r="O22">
         <f t="shared" ref="O22:O85" ca="1" si="1">SQRT((L22-$L$12)^2+(M22-$M$12)^2)</f>
-        <v>1.8857479789196998</v>
+        <v>1.5916995822075442</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -1158,7 +1170,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5472685370804657</v>
+        <v>2.0127325306658479</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -1199,7 +1211,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3859031350583542</v>
+        <v>4.3322769717549745</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
@@ -1240,7 +1252,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76157208457287884</v>
+        <v>2.2192539286887367</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -1281,7 +1293,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4479343907793669</v>
+        <v>2.4552663480775649</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -1322,7 +1334,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0038351458277366</v>
+        <v>1.4042261356350929</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -1363,7 +1375,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1268945647220032</v>
+        <v>1.7941826997268495</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -1404,7 +1416,7 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56269764527641208</v>
+        <v>1.7273708229560085</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
@@ -1445,7 +1457,7 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0087258050818106</v>
+        <v>2.9547590155546857</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -1486,7 +1498,7 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.411818575266766</v>
+        <v>3.1929979642966284</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
@@ -1527,7 +1539,7 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6926000000003114</v>
+        <v>3.0298612245447316</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -1568,7 +1580,7 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0407447525688858</v>
+        <v>1.2043496170130774</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
@@ -1609,7 +1621,7 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1457307537111787</v>
+        <v>1.4625682753291522</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
@@ -1650,7 +1662,7 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2807044964217216</v>
+        <v>1.4009549029143968</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
@@ -1691,7 +1703,7 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3795957233911138</v>
+        <v>0.99038101758852659</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
@@ -1732,7 +1744,7 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5671274685922785</v>
+        <v>3.6425792455349311</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
@@ -1773,7 +1785,7 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3969125891441618</v>
+        <v>0.88443256385085534</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
@@ -1814,7 +1826,7 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9144844083583754</v>
+        <v>5.0112405889159071</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
@@ -1855,7 +1867,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0274440331303918</v>
+        <v>1.9023710363649275</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
@@ -1896,7 +1908,7 @@
       </c>
       <c r="O41">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8438369573514524</v>
+        <v>2.4960260335177096</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -1937,7 +1949,7 @@
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7508560306318017</v>
+        <v>3.705991009163069</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
@@ -1978,7 +1990,7 @@
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="1"/>
-        <v>2.66129227256233</v>
+        <v>1.9668107077199275</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
@@ -2019,7 +2031,7 @@
       </c>
       <c r="O44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28158480072641123</v>
+        <v>2.3693914915016463</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
@@ -2060,7 +2072,7 @@
       </c>
       <c r="O45">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5311967028583924</v>
+        <v>3.4971238696959377</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -2101,7 +2113,7 @@
       </c>
       <c r="O46">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3222819820293896</v>
+        <v>1.9953979452729096</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
@@ -2142,7 +2154,7 @@
       </c>
       <c r="O47">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1457566932943699</v>
+        <v>1.9389312623193407</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
@@ -2183,7 +2195,7 @@
       </c>
       <c r="O48">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9335981899042767</v>
+        <v>1.3454823075766487</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
@@ -2224,7 +2236,7 @@
       </c>
       <c r="O49">
         <f t="shared" ca="1" si="1"/>
-        <v>2.968175196985587</v>
+        <v>5.0184499638830671</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
@@ -2265,7 +2277,7 @@
       </c>
       <c r="O50">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1676069385381505</v>
+        <v>0.66098136131030316</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
@@ -2306,7 +2318,7 @@
       </c>
       <c r="O51">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4571253919984368</v>
+        <v>2.868621648109094</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.35">
@@ -2347,7 +2359,7 @@
       </c>
       <c r="O52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65828531808054491</v>
+        <v>2.892051410331296</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.35">
@@ -2388,7 +2400,7 @@
       </c>
       <c r="O53">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9302775862556603</v>
+        <v>2.2544177430106775</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.35">
@@ -2429,7 +2441,7 @@
       </c>
       <c r="O54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27299999999922875</v>
+        <v>2.2106986768889447</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.35">
@@ -2470,7 +2482,7 @@
       </c>
       <c r="O55">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1855371980247438</v>
+        <v>3.3503382157628216</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.35">
@@ -2511,7 +2523,7 @@
       </c>
       <c r="O56">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7615494202546635</v>
+        <v>0.59363503939671214</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.35">
@@ -2552,7 +2564,7 @@
       </c>
       <c r="O57">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2737171166729757</v>
+        <v>1.1108087324107958</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.35">
@@ -2593,7 +2605,7 @@
       </c>
       <c r="O58">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2408348533522879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.35">
@@ -2634,7 +2646,7 @@
       </c>
       <c r="O59">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4980630354528448</v>
+        <v>2.6532976915535356</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.35">
@@ -2675,7 +2687,7 @@
       </c>
       <c r="O60">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0041578786738077</v>
+        <v>4.9101937273384841</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.35">
@@ -2716,7 +2728,7 @@
       </c>
       <c r="O61">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7126383856495169</v>
+        <v>0.98765631674197563</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.35">
@@ -2757,7 +2769,7 @@
       </c>
       <c r="O62">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9065735062836708</v>
+        <v>4.4104775659783719</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
@@ -2798,7 +2810,7 @@
       </c>
       <c r="O63">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3834269529394234</v>
+        <v>3.7810125310552749</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.35">
@@ -2839,7 +2851,7 @@
       </c>
       <c r="O64">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6720794359124713</v>
+        <v>3.694913801430566</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.35">
@@ -2880,7 +2892,7 @@
       </c>
       <c r="O65">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8613801373678758</v>
+        <v>2.6226950566162119</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
@@ -2921,7 +2933,7 @@
       </c>
       <c r="O66">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4471763320203244</v>
+        <v>2.7935995489691536</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.35">
@@ -2962,7 +2974,7 @@
       </c>
       <c r="O67">
         <f t="shared" ca="1" si="1"/>
-        <v>5.074470017646691</v>
+        <v>2.9916445243375391</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
@@ -3003,7 +3015,7 @@
       </c>
       <c r="O68">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1318542494821218</v>
+        <v>2.4608724062822969</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
@@ -3044,7 +3056,7 @@
       </c>
       <c r="O69">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93076110791056565</v>
+        <v>2.3415475651798121</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.35">
@@ -3085,7 +3097,7 @@
       </c>
       <c r="O70">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1615744495420484</v>
+        <v>1.658115388023103</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.35">
@@ -3126,7 +3138,7 @@
       </c>
       <c r="O71">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4648801862273391</v>
+        <v>3.5896613545014739</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.35">
@@ -3167,7 +3179,7 @@
       </c>
       <c r="O72">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.2408348533522879</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.35">
@@ -3208,7 +3220,7 @@
       </c>
       <c r="O73">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5021845975068535</v>
+        <v>1.4212758915849339</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.35">
@@ -3249,7 +3261,7 @@
       </c>
       <c r="O74">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2420000000001892</v>
+        <v>3.4711059966527604</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.35">
@@ -3290,7 +3302,7 @@
       </c>
       <c r="O75">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1501208245116996</v>
+        <v>0.60455054379331818</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.35">
@@ -3331,7 +3343,7 @@
       </c>
       <c r="O76">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1300263321577599</v>
+        <v>1.9704383674709913</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
@@ -3372,7 +3384,7 @@
       </c>
       <c r="O77">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0816244854219823</v>
+        <v>2.3880979879388451</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
@@ -3413,7 +3425,7 @@
       </c>
       <c r="O78">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9607603360970542</v>
+        <v>3.9460139381405548</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">
@@ -3454,7 +3466,7 @@
       </c>
       <c r="O79">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5412921201620602</v>
+        <v>1.100685241110827</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
@@ -3495,7 +3507,7 @@
       </c>
       <c r="O80">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5401007273797394</v>
+        <v>1.4654090759914609</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.35">
@@ -3536,7 +3548,7 @@
       </c>
       <c r="O81">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9342373797214418</v>
+        <v>1.7169321594053044</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.35">
@@ -3577,7 +3589,7 @@
       </c>
       <c r="O82">
         <f t="shared" ca="1" si="1"/>
-        <v>3.668521685910846</v>
+        <v>1.7941826997271992</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.35">
@@ -3618,7 +3630,7 @@
       </c>
       <c r="O83">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2807044964217216</v>
+        <v>2.1134921433494473</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.35">
@@ -3659,7 +3671,7 @@
       </c>
       <c r="O84">
         <f t="shared" ca="1" si="1"/>
-        <v>5.660370521441064</v>
+        <v>3.4569059229319175</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.35">
@@ -3700,7 +3712,7 @@
       </c>
       <c r="O85">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9393669318401567</v>
+        <v>1.1132281706816745</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
@@ -3741,7 +3753,7 @@
       </c>
       <c r="O86">
         <f t="shared" ref="O86:O115" ca="1" si="2">SQRT((L86-$L$12)^2+(M86-$M$12)^2)</f>
-        <v>0.38191025123664191</v>
+        <v>1.8757578628386304</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.35">
@@ -3782,7 +3794,7 @@
       </c>
       <c r="O87">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5421581680780578</v>
+        <v>5.3929459259290526</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.35">
@@ -3823,7 +3835,7 @@
       </c>
       <c r="O88">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4996219523598344</v>
+        <v>2.9948517225395292</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.35">
@@ -3864,7 +3876,7 @@
       </c>
       <c r="O89">
         <f t="shared" ca="1" si="2"/>
-        <v>2.3049630018725673</v>
+        <v>4.0967280310023053</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.35">
@@ -3905,7 +3917,7 @@
       </c>
       <c r="O90">
         <f t="shared" ca="1" si="2"/>
-        <v>5.2131555472667026</v>
+        <v>4.0779328292652206</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
@@ -3946,7 +3958,7 @@
       </c>
       <c r="O91">
         <f t="shared" ca="1" si="2"/>
-        <v>3.2034153399149399</v>
+        <v>3.7829132107416461</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.35">
@@ -3987,7 +3999,7 @@
       </c>
       <c r="O92">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7164976642736667</v>
+        <v>4.3463924627216848</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.35">
@@ -4028,7 +4040,7 @@
       </c>
       <c r="O93">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7285103413053058</v>
+        <v>2.0783093225022116</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.35">
@@ -4069,7 +4081,7 @@
       </c>
       <c r="O94">
         <f t="shared" ca="1" si="2"/>
-        <v>2.991681707668735</v>
+        <v>3.887315726822258</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
@@ -4110,7 +4122,7 @@
       </c>
       <c r="O95">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1167794052537698</v>
+        <v>2.8812075593399626</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.35">
@@ -4151,7 +4163,7 @@
       </c>
       <c r="O96">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0707199617526078</v>
+        <v>4.290525114714745</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.35">
@@ -4192,7 +4204,7 @@
       </c>
       <c r="O97">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68903044925496215</v>
+        <v>2.8292504236990421</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
@@ -4233,7 +4245,7 @@
       </c>
       <c r="O98">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87571413143803378</v>
+        <v>2.9675023437228365</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.35">
@@ -4274,7 +4286,7 @@
       </c>
       <c r="O99">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2178878273473648</v>
+        <v>3.4547036110207499</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.35">
@@ -4315,7 +4327,7 @@
       </c>
       <c r="O100">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2467315460461967</v>
+        <v>0.93925606732119726</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.35">
@@ -4356,7 +4368,7 @@
       </c>
       <c r="O101">
         <f t="shared" ca="1" si="2"/>
-        <v>4.273828302587189</v>
+        <v>2.2418127843329096</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.35">
@@ -4397,7 +4409,7 @@
       </c>
       <c r="O102">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5715440031241537</v>
+        <v>3.9989596697144827</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.35">
@@ -4438,7 +4450,7 @@
       </c>
       <c r="O103">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0265399192682123</v>
+        <v>3.1711435539881241</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.35">
@@ -4479,7 +4491,7 @@
       </c>
       <c r="O104">
         <f t="shared" ca="1" si="2"/>
-        <v>4.6731451336329801</v>
+        <v>2.487962129936959</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
@@ -4520,7 +4532,7 @@
       </c>
       <c r="O105">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66098136131030316</v>
+        <v>1.9443051612334608</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
@@ -4561,7 +4573,7 @@
       </c>
       <c r="O106">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0741545265479373</v>
+        <v>0.95100170346876101</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
@@ -4602,7 +4614,7 @@
       </c>
       <c r="O107">
         <f t="shared" ca="1" si="2"/>
-        <v>2.3850670933961098</v>
+        <v>0.33478763418084051</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.35">
@@ -4643,7 +4655,7 @@
       </c>
       <c r="O108">
         <f t="shared" ca="1" si="2"/>
-        <v>3.598370881384755</v>
+        <v>1.3843137794591485</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.35">
@@ -4684,7 +4696,7 @@
       </c>
       <c r="O109">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3276599173228565</v>
+        <v>3.1312639364964419</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
@@ -4725,7 +4737,7 @@
       </c>
       <c r="O110">
         <f t="shared" ca="1" si="2"/>
-        <v>1.518981619374886</v>
+        <v>0.76382050247412614</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
@@ -4766,7 +4778,7 @@
       </c>
       <c r="O111">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1760082871422539</v>
+        <v>2.27656011561275</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.35">
@@ -4807,7 +4819,7 @@
       </c>
       <c r="O112">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3875756403731279</v>
+        <v>4.7708998773810976</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.35">
@@ -4848,7 +4860,7 @@
       </c>
       <c r="O113">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2968175196987789</v>
+        <v>2.4989567823393215</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
@@ -4889,7 +4901,7 @@
       </c>
       <c r="O114">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6271114251201606</v>
+        <v>0.68520945702763258</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.35">
@@ -4930,7 +4942,7 @@
       </c>
       <c r="O115">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4656084197354338</v>
+        <v>1.3714254482108088</v>
       </c>
     </row>
   </sheetData>
@@ -4950,10 +4962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9675C56-A66C-4392-BA99-E6320C858F8D}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5418,40 +5430,40 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="C12">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>13423</v>
+        <v>12059</v>
       </c>
       <c r="E12">
-        <v>13522</v>
+        <v>12158</v>
       </c>
       <c r="F12">
         <v>0.01</v>
       </c>
       <c r="G12">
-        <v>12.33</v>
+        <v>11.54</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="I12">
-        <v>12.13</v>
+        <v>11.38</v>
       </c>
       <c r="J12">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K12">
-        <v>3.62</v>
+        <v>3.01</v>
       </c>
       <c r="L12">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="M12">
-        <v>0.8</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -6243,8 +6255,38 @@
       <c r="C32">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>12757</v>
+      </c>
+      <c r="E32">
+        <v>12823</v>
+      </c>
+      <c r="F32">
+        <v>0.01</v>
+      </c>
+      <c r="G32">
+        <v>6.74</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>6.64</v>
+      </c>
+      <c r="J32">
+        <v>17</v>
+      </c>
+      <c r="K32">
+        <v>1.23</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6254,8 +6296,38 @@
       <c r="C33">
         <v>89</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>7198</v>
+      </c>
+      <c r="E33">
+        <v>7198</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>12.88</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>12.73</v>
+      </c>
+      <c r="J33">
+        <v>34</v>
+      </c>
+      <c r="K33">
+        <v>2.58</v>
+      </c>
+      <c r="L33">
+        <v>7</v>
+      </c>
+      <c r="M33">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6265,19 +6337,79 @@
       <c r="C34">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>9246</v>
+      </c>
+      <c r="E34">
+        <v>9246</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>47.36</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>47.16</v>
+      </c>
+      <c r="J34">
+        <v>215</v>
+      </c>
+      <c r="K34">
+        <v>17.03</v>
+      </c>
+      <c r="L34">
+        <v>65</v>
+      </c>
+      <c r="M34">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C35">
+        <v>41</v>
+      </c>
+      <c r="D35">
+        <v>10044</v>
+      </c>
+      <c r="E35">
+        <v>10131</v>
+      </c>
+      <c r="F35">
+        <v>0.01</v>
+      </c>
+      <c r="G35">
+        <v>84.58</v>
+      </c>
+      <c r="H35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="I35">
+        <v>84.4</v>
+      </c>
+      <c r="J35">
+        <v>117</v>
+      </c>
+      <c r="K35">
+        <v>10.46</v>
+      </c>
+      <c r="L35">
+        <v>3</v>
+      </c>
+      <c r="M35">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6287,8 +6419,38 @@
       <c r="C36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>10597</v>
+      </c>
+      <c r="E36">
+        <v>10684</v>
+      </c>
+      <c r="F36">
+        <v>0.01</v>
+      </c>
+      <c r="G36">
+        <v>8.17</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>7.98</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>0.72</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6298,8 +6460,38 @@
       <c r="C37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>11877</v>
+      </c>
+      <c r="E37">
+        <v>11879</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>13.44</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>13.26</v>
+      </c>
+      <c r="J37">
+        <v>16</v>
+      </c>
+      <c r="K37">
+        <v>1.43</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6309,8 +6501,38 @@
       <c r="C38">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>12135</v>
+      </c>
+      <c r="E38">
+        <v>12222</v>
+      </c>
+      <c r="F38">
+        <v>0.01</v>
+      </c>
+      <c r="G38">
+        <v>15.71</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>15.49</v>
+      </c>
+      <c r="J38">
+        <v>57</v>
+      </c>
+      <c r="K38">
+        <v>5.79</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6320,8 +6542,38 @@
       <c r="C39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>12460</v>
+      </c>
+      <c r="E39">
+        <v>12460</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>15.12</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>14.9</v>
+      </c>
+      <c r="J39">
+        <v>37</v>
+      </c>
+      <c r="K39">
+        <v>5.53</v>
+      </c>
+      <c r="L39">
+        <v>12</v>
+      </c>
+      <c r="M39">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6331,8 +6583,38 @@
       <c r="C40">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>9670</v>
+      </c>
+      <c r="E40">
+        <v>9670</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>8.9</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>8.74</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>0.68</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6342,8 +6624,38 @@
       <c r="C41">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>11222</v>
+      </c>
+      <c r="E41">
+        <v>11243</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>12.36</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>12.19</v>
+      </c>
+      <c r="J41">
+        <v>46</v>
+      </c>
+      <c r="K41">
+        <v>3.39</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6353,8 +6665,38 @@
       <c r="C42">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>7351</v>
+      </c>
+      <c r="E42">
+        <v>7352</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>45.94</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>45.75</v>
+      </c>
+      <c r="J42">
+        <v>283</v>
+      </c>
+      <c r="K42">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6364,8 +6706,38 @@
       <c r="C43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>11258</v>
+      </c>
+      <c r="E43">
+        <v>11261</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>12.51</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>12.33</v>
+      </c>
+      <c r="J43">
+        <v>28</v>
+      </c>
+      <c r="K43">
+        <v>3.2</v>
+      </c>
+      <c r="L43">
+        <v>3</v>
+      </c>
+      <c r="M43">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6375,8 +6747,38 @@
       <c r="C44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>11455</v>
+      </c>
+      <c r="E44">
+        <v>11542</v>
+      </c>
+      <c r="F44">
+        <v>0.01</v>
+      </c>
+      <c r="G44">
+        <v>10.01</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>9.86</v>
+      </c>
+      <c r="J44">
+        <v>21</v>
+      </c>
+      <c r="K44">
+        <v>1.84</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6386,8 +6788,38 @@
       <c r="C45">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>13120</v>
+      </c>
+      <c r="E45">
+        <v>13186</v>
+      </c>
+      <c r="F45">
+        <v>0.01</v>
+      </c>
+      <c r="G45">
+        <v>10.28</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="J45">
+        <v>19</v>
+      </c>
+      <c r="K45">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L45">
+        <v>6</v>
+      </c>
+      <c r="M45">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6397,8 +6829,38 @@
       <c r="C46">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>8903</v>
+      </c>
+      <c r="E46">
+        <v>8903</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>58.34</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>58.18</v>
+      </c>
+      <c r="J46">
+        <v>732</v>
+      </c>
+      <c r="K46">
+        <v>44.55</v>
+      </c>
+      <c r="L46">
+        <v>101</v>
+      </c>
+      <c r="M46">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6408,8 +6870,38 @@
       <c r="C47">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>6640</v>
+      </c>
+      <c r="E47">
+        <v>6641</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>12.15</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>11.9</v>
+      </c>
+      <c r="J47">
+        <v>22</v>
+      </c>
+      <c r="K47">
+        <v>1.8</v>
+      </c>
+      <c r="L47">
+        <v>14</v>
+      </c>
+      <c r="M47">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6419,8 +6911,38 @@
       <c r="C48">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>9035</v>
+      </c>
+      <c r="E48">
+        <v>9035</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>30.22</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>29.94</v>
+      </c>
+      <c r="J48">
+        <v>93</v>
+      </c>
+      <c r="K48">
+        <v>8.15</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6430,8 +6952,38 @@
       <c r="C49">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>9522</v>
+      </c>
+      <c r="E49">
+        <v>9524</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>25.42</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>25.21</v>
+      </c>
+      <c r="J49">
+        <v>92</v>
+      </c>
+      <c r="K49">
+        <v>5.13</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6441,8 +6993,38 @@
       <c r="C50">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <v>11885</v>
+      </c>
+      <c r="E50">
+        <v>11972</v>
+      </c>
+      <c r="F50">
+        <v>0.01</v>
+      </c>
+      <c r="G50">
+        <v>13.62</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>13.46</v>
+      </c>
+      <c r="J50">
+        <v>32</v>
+      </c>
+      <c r="K50">
+        <v>5.03</v>
+      </c>
+      <c r="L50">
+        <v>3</v>
+      </c>
+      <c r="M50">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6451,6 +7033,72 @@
       </c>
       <c r="C51">
         <v>74</v>
+      </c>
+      <c r="D51">
+        <v>10178</v>
+      </c>
+      <c r="E51">
+        <v>10178</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>26.9</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>26.71</v>
+      </c>
+      <c r="J51">
+        <v>57</v>
+      </c>
+      <c r="K51">
+        <v>9.32</v>
+      </c>
+      <c r="L51">
+        <v>6</v>
+      </c>
+      <c r="M51">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54">
+        <f>AVERAGE(E2:E51)</f>
+        <v>10019.24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55">
+        <f>MAX(E2:E51)</f>
+        <v>13401</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56">
+        <f>MIN(E2:E51)</f>
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57">
+        <f>_xlfn.STDEV.P(E2:E51)</f>
+        <v>2561.5910021703307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
50 simulated tornado results for 30M
</commit_message>
<xml_diff>
--- a/Results/20231224 Revision_Simulated_Tornado_15M.xlsx
+++ b/Results/20231224 Revision_Simulated_Tornado_15M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524CC5E4-D693-4D95-944F-1086A736CA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6789A7FD-B081-4C5A-8307-CC6CC710D194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,15 +769,15 @@
       </c>
       <c r="K11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="L11">
         <f ca="1">INDEX(Table1[coordinate_x],MATCH(K11,Table1[Block ID],0))</f>
-        <v>-94.504999999999995</v>
+        <v>-94.542000000000002</v>
       </c>
       <c r="M11">
         <f ca="1">INDEX(Table1[coordinate_y],MATCH(K11,Table1[Block ID],0))</f>
-        <v>37.091999999999999</v>
+        <v>37.082999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -795,11 +795,11 @@
       </c>
       <c r="L12">
         <f ca="1">L11*54.6</f>
-        <v>-5159.973</v>
+        <v>-5161.9931999999999</v>
       </c>
       <c r="M12">
         <f ca="1">M11*69</f>
-        <v>2559.348</v>
+        <v>2558.7269999999999</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -883,7 +883,7 @@
       </c>
       <c r="O16">
         <f ca="1">SQRT((L16-$L$12)^2+(M16-$M$12)^2)</f>
-        <v>1.4985585874433502</v>
+        <v>2.5410843669582648</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -924,7 +924,7 @@
       </c>
       <c r="O17">
         <f ca="1">SQRT((L17-$L$12)^2+(M17-$M$12)^2)</f>
-        <v>1.0558745380016294</v>
+        <v>2.6833960125185374</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -965,7 +965,7 @@
       </c>
       <c r="O18">
         <f t="shared" ref="O18:O19" ca="1" si="0">SQRT((L18-$L$12)^2+(M18-$M$12)^2)</f>
-        <v>1.3799999999996544</v>
+        <v>2.158075309158384</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8474569007152806</v>
+        <v>1.5855934031139691</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="O20">
         <f ca="1">SQRT((L20-$L$12)^2+(M20-$M$12)^2)</f>
-        <v>3.4769380840045288</v>
+        <v>1.8093482251904933</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="O21">
         <f ca="1">SQRT((L21-$L$12)^2+(M21-$M$12)^2)</f>
-        <v>2.1997386208369334</v>
+        <v>1.2837846548384175</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="O22">
         <f t="shared" ref="O22:O85" ca="1" si="1">SQRT((L22-$L$12)^2+(M22-$M$12)^2)</f>
-        <v>1.5916995822075442</v>
+        <v>3.203421801761285</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0127325306658479</v>
+        <v>3.8319525049249763</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3322769717549745</v>
+        <v>2.3145262668631279</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2192539286887367</v>
+        <v>1.6063238278747052</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4552663480775649</v>
+        <v>1.1372532699443731</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4042261356350929</v>
+        <v>1.4996219523598344</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7941826997268495</v>
+        <v>1.1572631334312655</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7273708229560085</v>
+        <v>1.846199999999957</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9547590155546857</v>
+        <v>1.2178878273469269</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -1498,7 +1498,7 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1929979642966284</v>
+        <v>1.2550063904221633</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0298612245447316</v>
+        <v>1.5879389660810532</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2043496170130774</v>
+        <v>1.8323241634598733</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4625682753291522</v>
+        <v>1.2725547375259449</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4009549029143968</v>
+        <v>3.2759999999998399</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99038101758852659</v>
+        <v>2.2650286885596884</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6425792455349311</v>
+        <v>1.7792917804566577</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88443256385085534</v>
+        <v>1.3750536571349141</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0112405889159071</v>
+        <v>6.7255503863993091</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9023710363649275</v>
+        <v>3.8215105966097118</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="O41">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4960260335177096</v>
+        <v>4.2861015433604006</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="1"/>
-        <v>3.705991009163069</v>
+        <v>4.0107217106146829</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9668107077199275</v>
+        <v>0.55469375334511561</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="O44">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3693914915016463</v>
+        <v>2.1460570821856617</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="O45">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4971238696959377</v>
+        <v>5.5665872992341292</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="O46">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9953979452729096</v>
+        <v>3.1225001905521923</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="O47">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9389312623193407</v>
+        <v>3.1565851738861994</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="O48">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3454823075766487</v>
+        <v>0.77675695040260084</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="O49">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0184499638830671</v>
+        <v>5.1331578000286981</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="O50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66098136131030316</v>
+        <v>2.6434102292301418</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="O51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.868621648109094</v>
+        <v>4.9790556695019941</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.35">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="O52">
         <f t="shared" ca="1" si="1"/>
-        <v>2.892051410331296</v>
+        <v>2.6249815542201951</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.35">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="O53">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2544177430106775</v>
+        <v>0.48607629030808819</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.35">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="O54">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2106986768889447</v>
+        <v>2.4840471010017642</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.35">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="O55">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3503382157628216</v>
+        <v>4.9627277821778</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.35">
@@ -2523,7 +2523,7 @@
       </c>
       <c r="O56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59363503939671214</v>
+        <v>2.2396631353841179</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.35">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="O57">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1108087324107958</v>
+        <v>3.0760509033500281</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.35">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="O58">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.1134921433494473</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.35">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="O59">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6532976915535356</v>
+        <v>4.6456140605957446</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.35">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="O60">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9101937273384841</v>
+        <v>5.2456665887179321</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.35">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="O61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98765631674197563</v>
+        <v>1.2031801361387648</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.35">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="O62">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4104775659783719</v>
+        <v>5.8903067118780292</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="O63">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7810125310552749</v>
+        <v>4.6262818591168591</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.35">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="O64">
         <f t="shared" ca="1" si="1"/>
-        <v>3.694913801430566</v>
+        <v>2.7180062251586916</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.35">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="O65">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6226950566162119</v>
+        <v>4.1161715999212474</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="O66">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7935995489691536</v>
+        <v>0.72897530822383227</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.35">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="O67">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9916445243375391</v>
+        <v>4.8817124618311416</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
@@ -3015,7 +3015,7 @@
       </c>
       <c r="O68">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4608724062822969</v>
+        <v>0.87571413143809329</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="O69">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3415475651798121</v>
+        <v>3.0541313724193713</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.35">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="O70">
         <f t="shared" ca="1" si="1"/>
-        <v>1.658115388023103</v>
+        <v>1.4840875984929607</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.35">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="O71">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5896613545014739</v>
+        <v>3.6520450928212473</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.35">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="O72">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2408348533522879</v>
+        <v>2.2807044964217216</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.35">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="O73">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4212758915849339</v>
+        <v>0.91477885852287422</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.35">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="O74">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4711059966527604</v>
+        <v>3.2689883756290987</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.35">
@@ -3302,7 +3302,7 @@
       </c>
       <c r="O75">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60455054379331818</v>
+        <v>1.5231441691442271</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.35">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="O76">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9704383674709913</v>
+        <v>4.0149583609301862</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="O77">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3880979879388451</v>
+        <v>4.4937586317018452</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="O78">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9460139381405548</v>
+        <v>5.6775703113214355</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="O79">
         <f t="shared" ca="1" si="1"/>
-        <v>1.100685241110827</v>
+        <v>3.1494567531556172</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="O80">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4654090759914609</v>
+        <v>3.4772480153125169</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.35">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="O81">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7169321594053044</v>
+        <v>3.4688656878006685</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.35">
@@ -3589,7 +3589,7 @@
       </c>
       <c r="O82">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7941826997271992</v>
+        <v>2.1833868095233688</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.35">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="O83">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1134921433494473</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.35">
@@ -3671,7 +3671,7 @@
       </c>
       <c r="O84">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4569059229319175</v>
+        <v>4.451912425015081</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.35">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="O85">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1132281706816745</v>
+        <v>1.7416694749576567</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="O86">
         <f t="shared" ref="O86:O115" ca="1" si="2">SQRT((L86-$L$12)^2+(M86-$M$12)^2)</f>
-        <v>1.8757578628386304</v>
+        <v>2.1883891884217341</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.35">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="O87">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3929459259290526</v>
+        <v>7.2270956656178047</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.35">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="O88">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9948517225395292</v>
+        <v>3.7273681063179915</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.35">
@@ -3876,7 +3876,7 @@
       </c>
       <c r="O89">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0967280310023053</v>
+        <v>4.5823537881747098</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.35">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="O90">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0779328292652206</v>
+        <v>6.1730706589183031</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="O91">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7829132107416461</v>
+        <v>1.6908133072582623</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.35">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="O92">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3463924627216848</v>
+        <v>2.7637042099328553</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.35">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="O93">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0783093225022116</v>
+        <v>3.4356078064876163</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.35">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="O94">
         <f t="shared" ca="1" si="2"/>
-        <v>3.887315726822258</v>
+        <v>5.1030311815623604</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="O95">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8812075593399626</v>
+        <v>3.3853576531874383</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.35">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="O96">
         <f t="shared" ca="1" si="2"/>
-        <v>4.290525114714745</v>
+        <v>4.0297076519269792</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.35">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="O97">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8292504236990421</v>
+        <v>2.3663456129654343</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="O98">
         <f t="shared" ca="1" si="2"/>
-        <v>2.9675023437228365</v>
+        <v>3.1318542494818598</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.35">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="O99">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4547036110207499</v>
+        <v>3.0552820098964837</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.35">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="O100">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93925606732119726</v>
+        <v>2.9069321354306106</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.35">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="O101">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2418127843329096</v>
+        <v>4.2262509343384327</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.35">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="O102">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9989596697144827</v>
+        <v>2.3105189806621351</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.35">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="O103">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1711435539881241</v>
+        <v>5.2158720229699753</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.35">
@@ -4491,7 +4491,7 @@
       </c>
       <c r="O104">
         <f t="shared" ca="1" si="2"/>
-        <v>2.487962129936959</v>
+        <v>4.2463941456252972</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
@@ -4532,7 +4532,7 @@
       </c>
       <c r="O105">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9443051612334608</v>
+        <v>2.5942341760137539</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="O106">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95100170346876101</v>
+        <v>1.1678441676865108</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
@@ -4614,7 +4614,7 @@
       </c>
       <c r="O107">
         <f t="shared" ca="1" si="2"/>
-        <v>0.33478763418084051</v>
+        <v>2.4470931408515839</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.35">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="O108">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3843137794591485</v>
+        <v>2.7669336818936521</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.35">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="O109">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1312639364964419</v>
+        <v>5.2225171861856943</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
@@ -4737,7 +4737,7 @@
       </c>
       <c r="O110">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76382050247412614</v>
+        <v>1.694005832339738</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="O111">
         <f t="shared" ca="1" si="2"/>
-        <v>2.27656011561275</v>
+        <v>4.2638276747538271</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.35">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="O112">
         <f t="shared" ca="1" si="2"/>
-        <v>4.7708998773810976</v>
+        <v>6.3305637189741502</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.35">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="O113">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4989567823393215</v>
+        <v>2.5541097940375703</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
@@ -4901,7 +4901,7 @@
       </c>
       <c r="O114">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68520945702763258</v>
+        <v>1.8012469680748062</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.35">
@@ -4942,7 +4942,7 @@
       </c>
       <c r="O115">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3714254482108088</v>
+        <v>1.0208192004461221</v>
       </c>
     </row>
   </sheetData>
@@ -4964,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9675C56-A66C-4392-BA99-E6320C858F8D}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>